<commit_message>
20221208_V2.5.8 add TxBW Tx MPD X and Y monitor
</commit_message>
<xml_diff>
--- a/Configuration/test_report_TxBW.xlsx
+++ b/Configuration/test_report_TxBW.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test_script\FS400_Final_Test_Desk1\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jiawen_zhou\FS400_Final_test\FS400_Final_Test_Desk1\Configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E08FB2-191B-49D2-A0AF-E3BDD2149D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27840" yWindow="960" windowWidth="21750" windowHeight="13680"/>
+    <workbookView xWindow="-25830" yWindow="1560" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Result" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -24,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>SN</t>
   </si>
@@ -183,13 +185,21 @@
   </si>
   <si>
     <t>amp_Imbalance</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Res_TxMPDX</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Res_TxMPDY</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -819,7 +829,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -855,6 +865,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - 着色 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1406,24 +1419,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="15.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.75" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" style="2" customWidth="1"/>
     <col min="7" max="7" width="9" style="2"/>
-    <col min="9" max="9" width="10.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1433,7 +1446,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -1443,7 +1456,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1453,7 +1466,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1463,7 +1476,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
@@ -1473,7 +1486,7 @@
       </c>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1486,7 +1499,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
@@ -1509,7 +1522,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
@@ -1535,7 +1548,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>14</v>
       </c>
@@ -1561,7 +1574,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>15</v>
       </c>
@@ -1587,7 +1600,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>16</v>
       </c>
@@ -1615,7 +1628,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>17</v>
       </c>
@@ -1639,7 +1652,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>18</v>
       </c>
@@ -1665,7 +1678,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>19</v>
       </c>
@@ -1691,7 +1704,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>20</v>
       </c>
@@ -1717,7 +1730,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>21</v>
       </c>
@@ -1745,7 +1758,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>22</v>
       </c>
@@ -1769,7 +1782,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>23</v>
       </c>
@@ -1795,7 +1808,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>24</v>
       </c>
@@ -1821,7 +1834,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>25</v>
       </c>
@@ -1847,7 +1860,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>26</v>
       </c>
@@ -1875,7 +1888,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>27</v>
       </c>
@@ -1899,7 +1912,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>28</v>
       </c>
@@ -1925,7 +1938,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>29</v>
       </c>
@@ -1951,7 +1964,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>30</v>
       </c>
@@ -1977,7 +1990,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>31</v>
       </c>
@@ -2005,7 +2018,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>32</v>
       </c>
@@ -2029,7 +2042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>40</v>
       </c>
@@ -2055,7 +2068,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>41</v>
       </c>
@@ -2081,7 +2094,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>42</v>
       </c>
@@ -2107,7 +2120,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>43</v>
       </c>
@@ -2133,7 +2146,7 @@
         <v>Fail</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>44</v>
       </c>
@@ -2161,6 +2174,32 @@
         <f t="shared" si="19"/>
         <v>Fail</v>
       </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>

<commit_message>
20221208_V2.5.9: 1.Update report model; 2.Fixed noipwr bug;
</commit_message>
<xml_diff>
--- a/Configuration/test_report_TxBW.xlsx
+++ b/Configuration/test_report_TxBW.xlsx
@@ -1418,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1487,7 +1487,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="str">
-        <f>IF(SUM(H8:H33)=23,"Pass","Fail")</f>
+        <f>IF(SUM(H8:H34)=23,"Pass","Fail")</f>
         <v>Fail</v>
       </c>
       <c r="C6" s="4" t="s">

</xml_diff>